<commit_message>
Added E2E demo test cases excel sheet, Updated ItemDescriptionPage class
</commit_message>
<xml_diff>
--- a/RetailWebsite-TestCasesForAutomation.xlsx
+++ b/RetailWebsite-TestCasesForAutomation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DB4257-FC29-4D89-AAC3-99872270D717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F2B210-8C3E-4ECD-8E50-A5062CE573BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{6FFB5DF8-F707-4215-9954-B122C430142A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6FFB5DF8-F707-4215-9954-B122C430142A}"/>
   </bookViews>
   <sheets>
     <sheet name="Project details" sheetId="1" r:id="rId1"/>
@@ -484,15 +484,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,9 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170DE5D6-E46C-4FD0-925A-5A9F4E78B0E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -845,7 +845,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -857,7 +857,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -869,7 +869,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -881,7 +881,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -893,7 +893,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>75</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -905,7 +905,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -917,7 +917,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -929,7 +929,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -941,7 +941,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1137,7 +1137,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1157,7 +1157,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
@@ -1431,9 +1431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707D2BE4-5CAF-40AC-88BE-07130274224A}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1444,20 +1444,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1465,10 +1465,10 @@
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1476,10 +1476,10 @@
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1487,10 +1487,10 @@
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1498,10 +1498,10 @@
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1509,10 +1509,10 @@
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1520,10 +1520,10 @@
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1531,10 +1531,10 @@
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1542,10 +1542,10 @@
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committing test results. Renamed TC007_TC001 to TS007_TC001
</commit_message>
<xml_diff>
--- a/RetailWebsite-TestCasesForAutomation.xlsx
+++ b/RetailWebsite-TestCasesForAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F2B210-8C3E-4ECD-8E50-A5062CE573BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5041E01-7E8F-49FF-A66F-B284F41A1961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6FFB5DF8-F707-4215-9954-B122C430142A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{6FFB5DF8-F707-4215-9954-B122C430142A}"/>
   </bookViews>
   <sheets>
     <sheet name="Project details" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
 2. The stores near to the searched town or postcode should be displayed on the Stores near page.</t>
   </si>
   <si>
-    <t>TC007_TC001_Navigation to other Currys website</t>
-  </si>
-  <si>
     <t>Verify the successful navigation from Currys UK home page to Currys Business, Currys Ireland and PartMaster page</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>JAVA Selenium Webdriver</t>
+  </si>
+  <si>
+    <t>TS007_TC001_Navigation to other Currys website</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170DE5D6-E46C-4FD0-925A-5A9F4E78B0E0}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -846,10 +846,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -858,10 +858,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -870,10 +870,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -882,10 +882,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -894,10 +894,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -906,10 +906,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -918,10 +918,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -930,10 +930,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -942,10 +942,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1082,8 +1082,8 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,7 +1098,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1118,16 +1118,16 @@
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -1138,65 +1138,65 @@
     </row>
     <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -1205,7 +1205,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
@@ -1216,16 +1216,16 @@
     </row>
     <row r="7" spans="1:6" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>17</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="8" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>15</v>
@@ -1245,7 +1245,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>19</v>
@@ -1256,22 +1256,22 @@
     </row>
     <row r="9" spans="1:6" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1431,9 +1431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707D2BE4-5CAF-40AC-88BE-07130274224A}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,7 +1448,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="10"/>
     </row>
@@ -1458,51 +1458,51 @@
         <v>9</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1510,21 +1510,21 @@
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1532,21 +1532,21 @@
         <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>